<commit_message>
Update Excel files and add questionnaire docx
Update binary Excel files data/Amenanzas.xlsx and data/CUESTIONARIO.xlsx, and add a new data/Questionario.docx (questionnaire document). These are binary/content updates, so changes are not viewable in a text diff.
</commit_message>
<xml_diff>
--- a/data/CUESTIONARIO.xlsx
+++ b/data/CUESTIONARIO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29628"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yyu3m\Desktop\Espacio compartida\SDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f6a2ed62d12d53eb/Documents/GitHub/SDA_Ver3/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E7B767-BA6B-4276-940F-DD6E4D4F156D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{37E7B767-BA6B-4276-940F-DD6E4D4F156D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D43ECDE-37EE-4902-94E1-A4629FE77899}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="E" sheetId="6" state="hidden" r:id="rId1"/>
@@ -2190,7 +2190,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2203,7 +2203,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2216,7 +2216,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2227,60 +2227,60 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="B1:G87"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A95" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55:D55"/>
+    <sheetView showFormulas="1" showGridLines="0" tabSelected="1" topLeftCell="A68" zoomScale="95" zoomScaleNormal="95" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37:D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="46.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="73.5546875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="2.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="58" t="s">
         <v>30</v>
       </c>
       <c r="C1" s="58"/>
       <c r="D1" s="59"/>
     </row>
-    <row r="2" spans="2:5" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="70" t="s">
         <v>37</v>
       </c>
       <c r="C2" s="70"/>
       <c r="D2" s="70"/>
     </row>
-    <row r="3" spans="2:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="10"/>
     </row>
-    <row r="4" spans="2:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="2:5" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="66"/>
       <c r="D5" s="67"/>
     </row>
-    <row r="6" spans="2:5" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="51"/>
       <c r="D6" s="51"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>24</v>
       </c>
@@ -2289,14 +2289,14 @@
       </c>
       <c r="D7" s="53"/>
     </row>
-    <row r="8" spans="2:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="51"/>
       <c r="D8" s="51"/>
     </row>
-    <row r="9" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>27</v>
       </c>
@@ -2306,7 +2306,7 @@
       <c r="D9" s="53"/>
       <c r="E9" s="15"/>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
         <v>28</v>
       </c>
@@ -2315,7 +2315,7 @@
       </c>
       <c r="D10" s="53"/>
     </row>
-    <row r="11" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>29</v>
       </c>
@@ -2325,14 +2325,14 @@
       <c r="D11" s="53"/>
       <c r="E11" s="15"/>
     </row>
-    <row r="12" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="13" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="51"/>
       <c r="D12" s="51"/>
     </row>
-    <row r="13" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
         <v>32</v>
       </c>
@@ -2342,7 +2342,7 @@
       <c r="D13" s="53"/>
       <c r="E13" s="15"/>
     </row>
-    <row r="14" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
         <v>39</v>
       </c>
@@ -2350,7 +2350,7 @@
       <c r="D14" s="51"/>
       <c r="E14" s="15"/>
     </row>
-    <row r="15" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
         <v>40</v>
       </c>
@@ -2360,7 +2360,7 @@
       <c r="D15" s="53"/>
       <c r="E15" s="15"/>
     </row>
-    <row r="16" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="s">
         <v>41</v>
       </c>
@@ -2370,7 +2370,7 @@
       <c r="D16" s="53"/>
       <c r="E16" s="15"/>
     </row>
-    <row r="17" spans="2:5" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
         <v>42</v>
       </c>
@@ -2380,7 +2380,7 @@
       <c r="D17" s="53"/>
       <c r="E17" s="15"/>
     </row>
-    <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="16" t="s">
         <v>23</v>
       </c>
@@ -2388,7 +2388,7 @@
       <c r="D18" s="57"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="16" t="s">
         <v>21</v>
       </c>
@@ -2396,7 +2396,7 @@
       <c r="D19" s="55"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="17" t="s">
         <v>22</v>
       </c>
@@ -2405,54 +2405,54 @@
       </c>
       <c r="D20" s="69"/>
     </row>
-    <row r="21" spans="2:5" ht="237" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" ht="237" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="74" t="s">
         <v>34</v>
       </c>
       <c r="C21" s="74"/>
       <c r="D21" s="74"/>
     </row>
-    <row r="22" spans="2:5" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" ht="23.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="11"/>
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
     </row>
-    <row r="23" spans="2:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="71" t="s">
         <v>31</v>
       </c>
       <c r="C23" s="72"/>
       <c r="D23" s="73"/>
     </row>
-    <row r="24" spans="2:5" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
       <c r="D24" s="19"/>
     </row>
-    <row r="25" spans="2:5" ht="154.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" ht="154.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="60" t="s">
         <v>47</v>
       </c>
       <c r="C25" s="61"/>
       <c r="D25" s="62"/>
     </row>
-    <row r="26" spans="2:5" ht="184.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" ht="184.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="63"/>
       <c r="C26" s="64"/>
       <c r="D26" s="65"/>
     </row>
-    <row r="27" spans="2:5" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="2:5" s="20" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" s="20" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="46" t="s">
         <v>48</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="48"/>
     </row>
-    <row r="29" spans="2:5" s="20" customFormat="1" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" s="20" customFormat="1" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
         <v>0</v>
       </c>
@@ -2461,19 +2461,19 @@
       </c>
       <c r="D29" s="50"/>
     </row>
-    <row r="30" spans="2:5" ht="123" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5" ht="123" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="43"/>
       <c r="C30" s="44"/>
       <c r="D30" s="45"/>
     </row>
-    <row r="31" spans="2:5" s="20" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:5" s="20" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="46" t="s">
         <v>49</v>
       </c>
       <c r="C31" s="47"/>
       <c r="D31" s="48"/>
     </row>
-    <row r="32" spans="2:5" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="21" t="s">
         <v>51</v>
       </c>
@@ -2483,7 +2483,7 @@
       <c r="D32" s="96"/>
       <c r="E32" s="22"/>
     </row>
-    <row r="33" spans="2:4" s="20" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" s="20" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
         <v>20</v>
       </c>
@@ -2492,19 +2492,19 @@
       </c>
       <c r="D33" s="94"/>
     </row>
-    <row r="34" spans="2:4" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:4" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="43"/>
       <c r="C34" s="44"/>
       <c r="D34" s="45"/>
     </row>
-    <row r="35" spans="2:4" s="20" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:4" s="20" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="46" t="s">
         <v>80</v>
       </c>
       <c r="C35" s="47"/>
       <c r="D35" s="48"/>
     </row>
-    <row r="36" spans="2:4" ht="195" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:4" ht="195" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="21" t="s">
         <v>54</v>
       </c>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="D36" s="96"/>
     </row>
-    <row r="37" spans="2:4" s="20" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" s="20" customFormat="1" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="7" t="s">
         <v>20</v>
       </c>
@@ -2522,19 +2522,19 @@
       </c>
       <c r="D37" s="94"/>
     </row>
-    <row r="38" spans="2:4" ht="93.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:4" ht="93.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="43"/>
       <c r="C38" s="44"/>
       <c r="D38" s="45"/>
     </row>
-    <row r="39" spans="2:4" s="20" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:4" s="20" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="46" t="s">
         <v>60</v>
       </c>
       <c r="C39" s="47"/>
       <c r="D39" s="48"/>
     </row>
-    <row r="40" spans="2:4" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:4" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="21" t="s">
         <v>57</v>
       </c>
@@ -2543,7 +2543,7 @@
       </c>
       <c r="D40" s="96"/>
     </row>
-    <row r="41" spans="2:4" s="20" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" s="20" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="7" t="s">
         <v>20</v>
       </c>
@@ -2552,26 +2552,26 @@
       </c>
       <c r="D41" s="94"/>
     </row>
-    <row r="42" spans="2:4" ht="101.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:4" ht="101.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="43"/>
       <c r="C42" s="44"/>
       <c r="D42" s="45"/>
     </row>
-    <row r="43" spans="2:4" s="20" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:4" s="20" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="46" t="s">
         <v>61</v>
       </c>
       <c r="C43" s="47"/>
       <c r="D43" s="48"/>
     </row>
-    <row r="44" spans="2:4" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:4" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="21"/>
       <c r="C44" s="95" t="s">
         <v>62</v>
       </c>
       <c r="D44" s="96"/>
     </row>
-    <row r="45" spans="2:4" s="20" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:4" s="20" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="7" t="s">
         <v>20</v>
       </c>
@@ -2580,26 +2580,26 @@
       </c>
       <c r="D45" s="94"/>
     </row>
-    <row r="46" spans="2:4" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:4" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="43"/>
       <c r="C46" s="44"/>
       <c r="D46" s="45"/>
     </row>
-    <row r="47" spans="2:4" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:4" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="71" t="s">
         <v>64</v>
       </c>
       <c r="C47" s="72"/>
       <c r="D47" s="73"/>
     </row>
-    <row r="48" spans="2:4" s="20" customFormat="1" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:4" s="20" customFormat="1" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="46" t="s">
         <v>65</v>
       </c>
       <c r="C48" s="97"/>
       <c r="D48" s="98"/>
     </row>
-    <row r="49" spans="2:7" s="20" customFormat="1" ht="91.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:7" s="20" customFormat="1" ht="91.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="23" t="s">
         <v>66</v>
       </c>
@@ -2609,7 +2609,7 @@
       <c r="D49" s="25"/>
       <c r="G49"/>
     </row>
-    <row r="50" spans="2:7" s="20" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:7" s="20" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="26" t="s">
         <v>11</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="51" spans="2:7" s="20" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:7" s="20" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="27" t="s">
         <v>19</v>
       </c>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="D51" s="101"/>
     </row>
-    <row r="52" spans="2:7" s="20" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:7" s="20" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="27" t="s">
         <v>1</v>
       </c>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="D52" s="101"/>
     </row>
-    <row r="53" spans="2:7" s="20" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:7" s="20" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="27" t="s">
         <v>13</v>
       </c>
@@ -2647,7 +2647,7 @@
       </c>
       <c r="D53" s="101"/>
     </row>
-    <row r="54" spans="2:7" s="20" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:7" s="20" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="28" t="s">
         <v>10</v>
       </c>
@@ -2656,19 +2656,19 @@
       </c>
       <c r="D54" s="102"/>
     </row>
-    <row r="55" spans="2:7" s="20" customFormat="1" ht="204" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:7" s="20" customFormat="1" ht="204" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="63"/>
       <c r="C55" s="64"/>
       <c r="D55" s="65"/>
     </row>
-    <row r="56" spans="2:7" s="20" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:7" s="20" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="46" t="s">
         <v>68</v>
       </c>
       <c r="C56" s="97"/>
       <c r="D56" s="98"/>
     </row>
-    <row r="57" spans="2:7" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:7" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="29" t="s">
         <v>69</v>
       </c>
@@ -2677,19 +2677,19 @@
       </c>
       <c r="D57" s="100"/>
     </row>
-    <row r="58" spans="2:7" ht="135" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:7" ht="135" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="63"/>
       <c r="C58" s="64"/>
       <c r="D58" s="65"/>
     </row>
-    <row r="59" spans="2:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="71" t="s">
         <v>35</v>
       </c>
       <c r="C59" s="72"/>
       <c r="D59" s="73"/>
     </row>
-    <row r="60" spans="2:7" ht="240.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:7" ht="240.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="30" t="s">
         <v>43</v>
       </c>
@@ -2698,12 +2698,12 @@
       </c>
       <c r="D60" s="100"/>
     </row>
-    <row r="61" spans="2:7" ht="227.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:7" ht="227.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="63"/>
       <c r="C61" s="64"/>
       <c r="D61" s="65"/>
     </row>
-    <row r="62" spans="2:7" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:7" ht="59.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="71" t="s">
         <v>38</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="2:7" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:7" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="91" t="s">
         <v>79</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="64" spans="2:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="92"/>
       <c r="C64" s="7"/>
       <c r="D64" s="32" t="s">
@@ -2731,21 +2731,21 @@
       </c>
       <c r="F64" s="42"/>
     </row>
-    <row r="65" spans="2:4" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:4" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="92"/>
       <c r="C65" s="7"/>
       <c r="D65" s="32" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="66" spans="2:4" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:4" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="92"/>
       <c r="C66" s="7"/>
       <c r="D66" s="32" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="67" spans="2:4" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:4" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="92"/>
       <c r="C67" s="7" t="s">
         <v>81</v>
@@ -2754,81 +2754,81 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="2:4" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:4" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="92"/>
       <c r="C68" s="7"/>
       <c r="D68" s="32" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="69" spans="2:4" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:4" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="92"/>
       <c r="C69" s="7"/>
       <c r="D69" s="32" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="70" spans="2:4" ht="98.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:4" ht="98.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="92"/>
       <c r="C70" s="5"/>
       <c r="D70" s="32" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="71" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="33" t="s">
         <v>6</v>
       </c>
       <c r="C71" s="87"/>
       <c r="D71" s="86"/>
     </row>
-    <row r="72" spans="2:4" ht="43.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:4" ht="43.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B72" s="34" t="s">
         <v>7</v>
       </c>
       <c r="C72" s="81"/>
       <c r="D72" s="82"/>
     </row>
-    <row r="73" spans="2:4" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:4" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="35"/>
     </row>
-    <row r="74" spans="2:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:4" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="88" t="s">
         <v>2</v>
       </c>
       <c r="C74" s="89"/>
       <c r="D74" s="90"/>
     </row>
-    <row r="75" spans="2:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="33" t="s">
         <v>9</v>
       </c>
       <c r="C75" s="85"/>
       <c r="D75" s="86"/>
     </row>
-    <row r="76" spans="2:4" ht="40.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:4" ht="40.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B76" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C76" s="81"/>
       <c r="D76" s="82"/>
     </row>
-    <row r="77" spans="2:4" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:4" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="37"/>
       <c r="C77" s="38"/>
       <c r="D77" s="38"/>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" s="39"/>
       <c r="C78" s="39"/>
     </row>
-    <row r="79" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B79" s="39"/>
       <c r="C79" s="39"/>
     </row>
-    <row r="80" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="77" t="s">
         <v>3</v>
       </c>
@@ -2837,49 +2837,49 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="83" t="s">
         <v>12</v>
       </c>
       <c r="C81" s="84"/>
       <c r="D81" s="3"/>
     </row>
-    <row r="82" spans="2:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="79" t="s">
         <v>4</v>
       </c>
       <c r="C82" s="80"/>
       <c r="D82" s="3"/>
     </row>
-    <row r="83" spans="2:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="79" t="s">
         <v>14</v>
       </c>
       <c r="C83" s="80"/>
       <c r="D83" s="3"/>
     </row>
-    <row r="84" spans="2:4" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:4" ht="58.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="79" t="s">
         <v>15</v>
       </c>
       <c r="C84" s="80"/>
       <c r="D84" s="3"/>
     </row>
-    <row r="85" spans="2:4" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:4" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B85" s="75" t="s">
         <v>33</v>
       </c>
       <c r="C85" s="76"/>
       <c r="D85" s="9"/>
     </row>
-    <row r="86" spans="2:4" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:4" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="75" t="s">
         <v>45</v>
       </c>
       <c r="C86" s="76"/>
       <c r="D86" s="9"/>
     </row>
-    <row r="87" spans="2:4" ht="43.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:4" ht="43.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B87" s="75" t="s">
         <v>46</v>
       </c>

</xml_diff>